<commit_message>
Aba de link da vaga
</commit_message>
<xml_diff>
--- a/vagas.xlsx
+++ b/vagas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Descrição</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -461,39 +466,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estágio de TI</t>
+          <t>Estágio em Infraestrutura de TI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fibra do Brasil</t>
+          <t>Timenow</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Vitória e Região</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Cargo: Estágio de TI Responsabilidades: Configurar e instalar softwares, servidores, roteadores, firewalls e outros dispositivos de rede. Monitorar o desempenho e a integridade da rede, firewall, notificar e aplicar as devidas correções. Resolver questões encaminhadas pelo suporte diagnosticando as infraestruturas local e de nuvem e solucionado seus problemas. Automatizar tarefas e monitorar sua eficácia. Criar, supervisionar e testar medidas de segurança (por exemplo, autenticação de acesso e recuperação de desastre). Comunicar-se com os usuários quando necessário. Manter documentação técnica completa. Sugerir melhorias de desempenho, capacidade e escalabilidade da rede. Projetar e implementar redes funcionais (LAN, WLAN, WAN). Demais atividades pertinentes ao setor. Competências Mínimo Exigido: Ensino superior cursando. Conhecimento em administração, configuração e otimização de Firewalls, roteadores, Switches, redes Wireless, IDS, IPS, Proxies e mecanismos de segurança em geral, além de conhecimento na estruturas de redes LAN, WAN e WLAN, segmentação, roteamento, protocolos e serviços (portas IP), VPN será um diferencial. Desejável: Saber trabalhar em equipe. Espirito de liderança. Ter excelente comunicação e relacionamento interpessoal. Vontade de crescer e se desenvolver dentro da empresa. Capacidade de organizar demandas. Ser atento aos detalhes e ser organizado. Ter comprometimento com prazos e qualidade. Perfil proativo, pontual, com senso analítico, de urgência e estratégico.
-Não informado
-A combinar
-Estagiário
-Fibra do Brasil
-Atua como distribuidora de produtos e matéria-prima para o corte industrial, produtos em metal duro (wideas) e produtos de embalagem e de proteção individual (EPIs).
-Máquinas/ Equipamentos/ Ferramentas
-Exibir mais
-Nível de experiência
-Estágio
-Tipo de emprego
-Tempo integral
-Função
-Tecnologia da informação
-Setores
-Fabricação de maquinário</t>
-        </is>
-      </c>
+          <t>Como você imagina o seu futuro? O que você deseja dele? E, mais importante, o que você está fazendo para que ele se torne possível?
+Há 26 anos temos engenhado um caminho que aponta para novos futuros possíveis, passando pela busca de uma realidade cada vez mais inclusiva, com garantia de respeito e equidade para todos.
+Neste ano, decidimos dar um passo à frente para mudarmos, de fato, a realidade. Afinal, o futuro é agora e queremos que você esteja nele conosco.
+Que tal ser um Time Player?
+O Time Players é o programa de estágio da Timenow. Por aqui, temos o compromisso de contribuir com a formação profissional e com o desenvolvimento de pessoas, além do incentivo à inovação e diversidade.
+.
+Então, se você quer trabalhar em um ambiente que incentiva o seu crescimento e experimentar a cultura de uma empresa que une a tradição da engenharia com a transformação provocada pela inovação, VEM SER TIME PLAYER! 💚
+Exibir mais
+Nível de experiência
+Não aplicável
+Tipo de emprego
+Tempo integral
+Função
+Educação e Treinamento
+Setores
+Fabricação de máquinas de automação</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -534,6 +540,7 @@
 Serviços de recursos humanos</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -541,102 +548,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Estágio de TI</t>
+          <t>Estágio para Cursos na área de tecnologia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Executiva Outsourcing</t>
+          <t>Up Estágio</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Brasília, DF</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
-        <is>
-          <t>Segunda a Sexta Feira das 08 as 14:15hrs - com 15min de intervalo
-Beneficios
-Formação Acadêmica:
-Não informado
-A combinar
-Estagiário
-EXECUTIVA OUTSOURCING
-Atividades de consultoria em gestão empresarial, exceto consultoria técnica específica
-Consultoria/ Auditoria
-Exibir mais
-Nível de experiência
-Estágio
-Tipo de emprego
-Tempo integral
-Função
-Tecnologia da informação
-Setores
-Serviços profissionais</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Estágio em Infraestrutura de TI</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Timenow</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Vitória e Região</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Como você imagina o seu futuro? O que você deseja dele? E, mais importante, o que você está fazendo para que ele se torne possível?
-Há 26 anos temos engenhado um caminho que aponta para novos futuros possíveis, passando pela busca de uma realidade cada vez mais inclusiva, com garantia de respeito e equidade para todos.
-Neste ano, decidimos dar um passo à frente para mudarmos, de fato, a realidade. Afinal, o futuro é agora e queremos que você esteja nele conosco.
-Que tal ser um Time Player?
-O Time Players é o programa de estágio da Timenow. Por aqui, temos o compromisso de contribuir com a formação profissional e com o desenvolvimento de pessoas, além do incentivo à inovação e diversidade.
-.
-Então, se você quer trabalhar em um ambiente que incentiva o seu crescimento e experimentar a cultura de uma empresa que une a tradição da engenharia com a transformação provocada pela inovação, VEM SER TIME PLAYER! 💚
-Exibir mais
-Nível de experiência
-Não aplicável
-Tipo de emprego
-Tempo integral
-Função
-Educação e Treinamento
-Setores
-Fabricação de máquinas de automação</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Estágio para Cursos na área de tecnologia</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Up Estágio</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Brasília, DF</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>ESTÁGIO PARA CURSOS NA ÁREA DE TECNOLOGIA 3 VAGA(S) ASA SUL Candidato Cursando: Estágio para Cursos na área de tecnologia 3 Vaga(s) A partir do 3 Semestre Local da Vaga: Asa Sul Carga Horária: 06 horas/dia de 08:00 às 14:00 ou de 12:00 às 18:00 ou à combinar Segunda à Sexta-feira Bolsa Auxílio: R$ 1.200,00 + Vale Transporte + Vale alimentação de R$ 930,00 por mês Atividades: Auxiliar projetos de tecnologia, monitoramento de sistemas e atividades correlatas com a área de TI. Inscreva-se em upestagio.com.br ou encaminhe o seu currículo para o email curriculosupestagio.com.br com o título: Estágio para Cursos na área de tecnologia - Asa Sul Requisitos: Ter conhecimentos em desenvolvimento, DBA, ORACLE, MYSQUL, redes, monitoramento de ativos em redes, microsoft, linux, AIX, inglês ou espanhol, noção de virtualização.
 Não informado
@@ -656,27 +581,28 @@
 Serviços profissionais</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Estágio de Suporte (TI) - Infraestrutura</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Zallpy Digital</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Porto Alegre e Região</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Job Description
 Transformar o futuro de pessoas e empresas com inovação e soluções digitais: esse é o nosso propósito.
@@ -712,27 +638,28 @@
 Tecnologia da informação e serviços</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Estágio de Suporte (TI) - Infraestrutura</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Ponyhof Leiting</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Porto Alegre, RS</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Transformar o futuro de pessoas e empresas com inovação e soluções digitais: esse é o nosso propósito.
 Suprimos as necessidades de desenvolvimento de produtos digitais customizados e com alto valor agregado, inovando em processos, ferramentas e conceitos. Aliamos tecnologias de alto desempenho e atuais no mercado com a expertise de uma equipe multidisciplinar formada por especialistas no segmento.
@@ -756,27 +683,28 @@
 Serviços e consultoria de TI</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Vagas de Estágio e Trainee abertas</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Matchbox</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>São Paulo e Região</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Você conhece a Comunidade Carreiras Matchbox? Não? Então aguenta aí que vou te explicar tu-di-nho A Comunidade Carreiras Matchbox nasceu com o objetivo de contribuir na jornada profissional de quem busca o mercado de trabalho, especialmente através de programas de estágio ou trainee. E nesse projeto temos três iniciativas: Comunidade / Chatbot, onde você responde algumas perguntinhas para mapearmos o seu perfil e recebe alertas sempre que surgir vagas em seu perfil. Além disso, membros da comunidade garantem um desconto exclusivo na Descomplica, o maior centro de ensino digital do Brasil com diversos cursos de graduação, pós e extensão para você turbinar a sua carreira. Aqui na Matchbox estamos com vagas abertas para: Programa de Estágio Sanofi Vagas Pontuais 2023 Graduate Program Schneider Electric 2023 - Trainee Agora convido você a fazer parte de nossa comunidade e vivenciar essa experiência. Tem amigos que possam ter interesse? Compartilhe também! Confira: https://bit.ly/3Jwc5dt
 Vale Transporte; Vale Refeição; Assistência Médica; Seguro de vida; Assistência Odontológica;
@@ -798,68 +726,71 @@
 Serviços profissionais</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Estágio Informática</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Tallentos Soluções</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>São Paulo e Região</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>s - Estágio Técnico em Análise de Sistemas - TI (Chance de efetivação) - CANOAS Auxiliar no desenvolvimento de sistema em linguagem de programação PHP; Testes nos sistemas desenvolvi VER MAIS
-Beneficios
-Não informado
-A combinar
-Estagiário
-Tallentos Soluções
-Empresa que atua no ramo de recursos humanos, sediada em Porto Alegre/RS.
-Recursos Humanos/ Recrutamento e seleção
-Exibir mais
-Nível de experiência
-Pleno-sênior
-Tipo de emprego
-Tempo integral
-Função
-Tecnologia da informação
-Setores
-Serviços de recursos humanos</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://br.linkedin.com/jobs/view/vagas-de-est%C3%A1gio-e-trainee-abertas-at-matchbox-3536485327?refId=iqcDgJHCjj2zwPxowMnP8w%3D%3D&amp;trackingId=ilVrzZSf9Ptwso5lpO38GA%3D%3D&amp;position=6&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Estágio em Governança de TI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Rockspoon do Brasil Sistemas de Informatica LTDA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>São Paulo, SP</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Como parte da equipe de Governança você contribuirá com a rotina de operações em uma startup multinacional. Inglês avançado é indispensável. Responsabilidades: Gestão da infraestrutura; Descrição de cenários testes; Execução de testes; Geração de métricas; Configurar métricas; Teste manual/automatizado; Apoio na criação e execução de CI/CD; Apoiar a criação de IaC (Infrastructure as Code). documentados, implementados e testados para integração. Produzir especificações técnicas detalhadas com base em documentos de requisitos de negócios. Garantir que padrões de projeto, metodologias e documentação de projeto consistentes sejam mantidos em todos os seus projetos de desenvolvimento. ? Trabalhar em estreita colaboração com os analistas de negócios e equipes de suporte para garantir que todos os requisitos técnicos para novos projetos sejam capturados, projetados e desenvolvidos de acordo com esses requisitos. ? Crie estratégias de engenharia de software que ajudem a identificar e mitigar riscos. Iniciativas diretas de melhoria de processos internos. Fornecer feedback sobre os processos, oferecendo sugestões.
+Exibir mais
+Nível de experiência
+Estágio
+Tipo de emprego
+Tempo integral
+Função
+Educação e Treinamento
+Setores
+Treinamento e suporte em sistemas de TI</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://br.linkedin.com/jobs/view/est%C3%A1gio-em-governan%C3%A7a-de-ti-at-rockspoon-do-brasil-sistemas-de-informatica-ltda-3537575548?refId=iqcDgJHCjj2zwPxowMnP8w%3D%3D&amp;trackingId=dpmI3KWmRnUU2%2Fz8xKQATg%3D%3D&amp;position=7&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Estágio em Compras Diretas - Niterói, RJ</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Baker Hughes</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Niterói, RJ</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Resumo da Função:
 Atuar com suporte a área de Sourcing Diretos, fazer controle de documentos de fornecedores para gate zero (certificados em avanço/green lights) realizando reuniões semanais para mostrar o andamento das atividades e apontando os que são críticos a operação solicitando suporte do time presente, acompanhar as datas de importação e pagamento das invoices junto a Logística Internacional e Finanças. Também prestar suporte logístico em relação ao processo de decisão dos modais de transporte quando necessário, sugerir e acompanhar as oportunidades de melhoria contínua e ser focal point de Sourcing para este tema, auxiliando na criação e desenvolvimento de KPIs e métricas de acompanhamento de desempenho semanal do time. Trabalhar em conjunto com os compradores na emissão e follow up das ordens de compra. Realizar treinamentos onlines pertinentes a área.
@@ -882,27 +813,77 @@
 Petróleo e gás</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Estágio Backoffice | Inclusão de pessoas com deficiência - São Paulo</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Mendes Talent</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>São Paulo, SP</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Somos uma consultoria especializada na atração de candidatos de todos os níveis e setores, e já atendemos a mais de 15 anos em todo o território nacional.
+Na Mendes Talent, valorizamos a diversidade e estamos comprometidos em oferecer as mesmas oportunidades de desenvolvimento para todas as pessoas independente de origem, raça, estado civil, idade, gênero, credo, cultura, classe social ou econômica, situação familiar, gravidez, idioma, orientação sexual, identidade de gênero, deficiência, doença, nacionalidade ou status migratório e/ou qualquer outro motivo.
+Todas as pessoas com deficiência podem se inscrever.
+VAGA: Estágio Backoffice
+Para trabalhar na Faculdade Sebrae, na Secretaria Acadêmica.
+Atendimento ao aluno, atendimento ao docente. Fará emissão de documentos, emissão de diploma.
+Habilidade com o Pacote Office.
+Escolaridade: Cursando ensino superior em Administração, Economia, Contabilidade, TI, Marketing, Engenharia.
+Desejável experiência em rotinas administrativas.
+Laudo Médico: O laudo médico deve estar atualizado.
+Disponibilidade para 30 horas semanais de jornada de trabalho.
+Seguro saúde Unimed
+Previdência privada complementar
+Auxílio-alimentação e/ou refeição
+Vale-transporte
+Exibir mais
+Nível de experiência
+Estágio
+Tipo de emprego
+Tempo integral
+Função
+Administração
+Setores
+Atendimento ao consumidor</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Estágio Superior de Tecnologia Gestao em TI</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Estágio Sul</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Porto Alegre, RS</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Cursando Técnico OU Superior em Análise e Desenvolvimento de Sistemas e áreas afins. Desejável conhecimento em PHP, CSS, HTML5, JavaScript, Bootstrap, MySQl. ATIVIDADES O estagiário auxiliará na atualização, desenvolvimento e programação de WebSites, intranet e extranet, lojas virtuais, manipulação de banco de dados e atualização de textos e imagens.
 Não informado
@@ -922,27 +903,32 @@
 Serviços de recursos humanos</t>
         </is>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://br.linkedin.com/jobs/view/est%C3%A1gio-superior-de-tecnologia-gestao-em-ti-at-est%C3%A1gio-sul-3536489746?refId=iqcDgJHCjj2zwPxowMnP8w%3D%3D&amp;trackingId=iSVJoUgZyuYHDuSDcqUnMw%3D%3D&amp;position=10&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>Estágio Superior de Tecnologia Gestao em TI</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Estágio Sul</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Porto Alegre, RS</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Cursando Análise e Desenvolvimento de Sistemas e áreas afins. Desejável conhecimento em Javascript, HTML e CSS3. ATIVIDADES O estagiário auxiliará a prover soluções técnicas para novas features e suporte a features já existentes, desenvolver interfaces responsivas mobile-first comprometendo-se com a usabilidade e fidelidade ao layout, integração de interface com APIs Rest (monolito / microsserviços). Auxiliará ativamente com UX Designer para garantir aderência do design à tecnologia adotada e aplicar boas práticas de codificação.
 Não informado
@@ -962,27 +948,32 @@
 Serviços de recursos humanos</t>
         </is>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://br.linkedin.com/jobs/view/est%C3%A1gio-superior-de-tecnologia-gestao-em-ti-at-est%C3%A1gio-sul-3536488986?refId=iqcDgJHCjj2zwPxowMnP8w%3D%3D&amp;trackingId=QkidixMYf04JD9TamMCDBw%3D%3D&amp;position=11&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Estágio Administracao enfase Gestao de TI</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Estágio Sul</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Porto Alegre, RS</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Atuará nas atividades internas e demais funções pertinentes ao cargo. Necessário experiência na área de atuação.
 Beneficios
@@ -1003,6 +994,51 @@
 Serviços de recursos humanos</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://br.linkedin.com/jobs/view/est%C3%A1gio-administracao-enfase-gestao-de-ti-at-est%C3%A1gio-sul-3536480054?refId=iqcDgJHCjj2zwPxowMnP8w%3D%3D&amp;trackingId=o%2F8wQryT%2Bblg2ETDrbSesg%3D%3D&amp;position=12&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Estágio Pós Vendas - Comercial</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>VERIBANK</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>São Paulo, SP</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Vaga de Estágio Pós Vendas - Comercial em São Paulo. A combinar. Período Integral. Estágio Área e especialização profissional: Comercial, Vendas - Atendimento Nível hierárquico: Estagiário Local de trabalho: São Paulo, SP Regime de contratação de tipo Estágio Jornada Período Integral Atribuições: Fidelização de clientes, acompanhamento da usabilidade do sistema, por meio de telefone, Anydesk, reuniões de atendimento via google meet.
+Requisitos: Ensino Superior cursando em administração, gestão comercial ou marketing, TI, Sistema da Informação, que tenham interesse na área comercial; Diferencial: Gostar de interagir com o público através de telefonema ou vídeo conferência, ser proativo, ter um bom relacionamento interpessoal.
+Exibir mais
+Nível de experiência
+Estágio
+Tipo de emprego
+Tempo integral
+Função
+Educação e Treinamento
+Setores
+Consultoria e serviços empresariais</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://br.linkedin.com/jobs/view/est%C3%A1gio-p%C3%B3s-vendas-comercial-at-veribank-3537570924?refId=iqcDgJHCjj2zwPxowMnP8w%3D%3D&amp;trackingId=hY3NSdlSeDPGB2A9PwFWMQ%3D%3D&amp;position=13&amp;pageNum=0&amp;trk=public_jobs_jserp-result_search-card</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>